<commit_message>
Update for first submission
</commit_message>
<xml_diff>
--- a/Meat substitutes/Data.xlsx
+++ b/Meat substitutes/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://feemit-my.sharepoint.com/personal/giacomo_falchetta_feem_it/Documents/Current papers/MEAT/Meat substitutes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://feemit-my.sharepoint.com/personal/giacomo_falchetta_feem_it/Documents/Current papers/MEAT/Repo/meatSSA/Meat substitutes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{1F2F0789-5FE1-4A6C-8281-EE063BF7EA08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{90FB4EC2-FBFE-4202-9370-CB82B306F467}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{1F2F0789-5FE1-4A6C-8281-EE063BF7EA08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{98D107D8-896F-4725-897E-60FB410BB58A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17DE93F0-18FA-4C4D-9E43-C81720BFA8DC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Type</t>
   </si>
@@ -139,16 +139,7 @@
     <t>75p_50a</t>
   </si>
   <si>
-    <t>Tempeh</t>
-  </si>
-  <si>
     <t>Pork</t>
-  </si>
-  <si>
-    <t>https://aip.scitation.org/doi/abs/10.1063/1.5064296</t>
-  </si>
-  <si>
-    <t>Poore and Nemcheck 2019</t>
   </si>
   <si>
     <t>Falafel</t>
@@ -176,6 +167,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -262,11 +256,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -274,8 +267,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C52E777-E988-4329-BF31-D6C5C1D0269F}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +611,7 @@
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -634,13 +630,13 @@
         <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -653,29 +649,29 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>4.38</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>4.2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <v>3.2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <v>48.79</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <v>3.32</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>140</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>280</v>
       </c>
       <c r="N2">
@@ -693,19 +689,19 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>3.5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>106.8</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <v>1.3</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>53.8</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>2.5</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -714,14 +710,14 @@
       <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>175</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>200</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N10" si="0">M3/L3</f>
+        <f t="shared" ref="N3:N8" si="0">M3/L3</f>
         <v>1.1428571428571428</v>
       </c>
     </row>
@@ -736,30 +732,30 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>7.3</v>
-      </c>
-      <c r="E4">
+        <v>23.9</v>
+      </c>
+      <c r="E4" s="6">
         <v>420</v>
       </c>
       <c r="F4" s="7">
         <v>5</v>
       </c>
-      <c r="G4">
-        <v>115</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
+      <c r="G4" s="6">
+        <v>291</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.4</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="5">
+        <v>41</v>
+      </c>
+      <c r="L4" s="4">
         <v>200</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>200</v>
       </c>
       <c r="N4">
@@ -777,28 +773,28 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>2.84</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>1.34</v>
       </c>
       <c r="F5" s="7">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <v>32</v>
       </c>
-      <c r="H5">
-        <v>2.84</v>
+      <c r="H5" s="6">
+        <v>1.5</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>200</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>200</v>
       </c>
       <c r="N5">
@@ -816,28 +812,28 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>3.59</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>0.95399999999999996</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>4.3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>39.700000000000003</v>
       </c>
-      <c r="H6">
-        <v>3.59</v>
+      <c r="H6" s="6">
+        <v>5.5</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>175</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>200</v>
       </c>
       <c r="N6">
@@ -847,7 +843,7 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -855,38 +851,41 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>2.65</v>
-      </c>
-      <c r="E7">
-        <v>0.73</v>
-      </c>
-      <c r="F7">
-        <v>5.6</v>
-      </c>
-      <c r="G7">
-        <v>27.78</v>
-      </c>
-      <c r="H7">
-        <v>2.65</v>
+      <c r="D7" s="6">
+        <v>5.55</v>
+      </c>
+      <c r="E7" s="6">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6">
+        <v>4</v>
+      </c>
+      <c r="G7" s="6">
+        <v>60.07</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.79</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="5">
-        <v>180</v>
-      </c>
-      <c r="M7" s="6">
+      <c r="K7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="4">
+        <v>140</v>
+      </c>
+      <c r="M7" s="5">
         <v>200</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>1.1111111111111112</v>
+        <v>1.4285714285714286</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -894,118 +893,72 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
-        <v>5.55</v>
-      </c>
-      <c r="E8">
-        <v>40</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>60.07</v>
-      </c>
-      <c r="H8">
-        <v>5.55</v>
+      <c r="D8" s="8">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>247</v>
+      </c>
+      <c r="F8" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="G8" s="8">
+        <v>12.2</v>
+      </c>
+      <c r="H8" s="8">
+        <v>4.43</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="5">
-        <v>140</v>
-      </c>
-      <c r="M8" s="6">
+        <v>37</v>
+      </c>
+      <c r="L8" s="4">
+        <v>130</v>
+      </c>
+      <c r="M8" s="5">
         <v>200</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>1.4285714285714286</v>
+        <v>1.5384615384615385</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="E9">
-        <v>7.18</v>
-      </c>
-      <c r="F9" s="7">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <f>0.3222+1.6</f>
-        <v>1.9222000000000001</v>
-      </c>
-      <c r="H9">
-        <v>3.5</v>
+      <c r="D9" s="6">
+        <v>2.65</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.73</v>
+      </c>
+      <c r="F9" s="6">
+        <v>5.6</v>
+      </c>
+      <c r="G9" s="6">
+        <v>27.78</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1.06</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="5">
-        <v>190</v>
-      </c>
-      <c r="M9" s="6">
-        <v>150</v>
+        <v>18</v>
+      </c>
+      <c r="L9" s="4">
+        <v>180</v>
+      </c>
+      <c r="M9" s="5">
+        <v>200</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
-        <v>0.78947368421052633</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.3280000000000001</v>
-      </c>
-      <c r="E10">
-        <v>224</v>
-      </c>
-      <c r="F10" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="G10" s="3">
-        <v>91.4</v>
-      </c>
-      <c r="H10" s="3">
-        <v>4.43</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="5">
-        <v>130</v>
-      </c>
-      <c r="M10" s="6">
-        <v>200</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="0"/>
-        <v>1.5384615384615385</v>
+        <f>M9/L9</f>
+        <v>1.1111111111111112</v>
       </c>
     </row>
   </sheetData>
@@ -1016,12 +969,11 @@
     <hyperlink ref="I4" r:id="rId4" display="https://sci-hub.tw/https:/link.springer.com/article/10.1007/s11367-015-0931-6" xr:uid="{F23F5967-2F10-45FD-A0DB-C58BE0726C08}"/>
     <hyperlink ref="I5" r:id="rId5" display="https://sci-hub.tw/https:/link.springer.com/article/10.1007/s11367-015-0931-6" xr:uid="{4C30CABF-188D-4129-8F5F-793C71735CE4}"/>
     <hyperlink ref="I6" r:id="rId6" display="https://sci-hub.tw/https:/link.springer.com/article/10.1007/s11367-015-0931-6" xr:uid="{49714C89-6D2A-4EFF-8F46-CA55204EEFB1}"/>
-    <hyperlink ref="I7" r:id="rId7" display="https://sci-hub.tw/https:/link.springer.com/article/10.1007/s11367-015-0931-6" xr:uid="{6CB0DB03-746C-40B9-9E45-C5189B4898FA}"/>
-    <hyperlink ref="I8" r:id="rId8" display="https://sci-hub.tw/https:/link.springer.com/article/10.1007/s11367-015-0931-6" xr:uid="{08BAAA37-92D2-4BF8-88E9-A5829AE095CF}"/>
-    <hyperlink ref="I9" r:id="rId9" xr:uid="{C0B11AAC-8A5D-4E35-B0EE-63C69E888E5D}"/>
-    <hyperlink ref="I10" r:id="rId10" xr:uid="{6E7433C9-2E21-4E4A-8033-BD08B0D07F65}"/>
-    <hyperlink ref="J4" r:id="rId11" display="https://www.gfi.org/images/uploads/2020/01/Cultivated-Meat-LCA-Report-2019-0709.pdf" xr:uid="{FA933BB9-F2F6-40F2-9BF0-DE365B1FE03D}"/>
-    <hyperlink ref="K8" r:id="rId12" xr:uid="{675A61B2-5FD8-4C3A-AA74-9DC45EC9AC09}"/>
+    <hyperlink ref="I9" r:id="rId7" display="https://sci-hub.tw/https:/link.springer.com/article/10.1007/s11367-015-0931-6" xr:uid="{6CB0DB03-746C-40B9-9E45-C5189B4898FA}"/>
+    <hyperlink ref="I7" r:id="rId8" display="https://sci-hub.tw/https:/link.springer.com/article/10.1007/s11367-015-0931-6" xr:uid="{08BAAA37-92D2-4BF8-88E9-A5829AE095CF}"/>
+    <hyperlink ref="I8" r:id="rId9" xr:uid="{6E7433C9-2E21-4E4A-8033-BD08B0D07F65}"/>
+    <hyperlink ref="J4" r:id="rId10" display="https://www.gfi.org/images/uploads/2020/01/Cultivated-Meat-LCA-Report-2019-0709.pdf" xr:uid="{FA933BB9-F2F6-40F2-9BF0-DE365B1FE03D}"/>
+    <hyperlink ref="K7" r:id="rId11" xr:uid="{675A61B2-5FD8-4C3A-AA74-9DC45EC9AC09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>